<commit_message>
- Nouveaux fichiers pour la région de morge aubonne
git-svn-id: https://svn.opac.ch/svn/cr/branches/vs2010.1@20539 787ff09c-d2b5-7842-b444-8dd0a418631d
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/App.Aider/Samples/EERV Région 2/id.xlsx
+++ b/Epsitec.Cresus/App.Aider/Samples/EERV Région 2/id.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>_id</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Gimel – Longirod</t>
+  </si>
+  <si>
+    <t>Région Morges-Aubonne</t>
   </si>
 </sst>
 </file>
@@ -469,10 +472,13 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="30.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -509,6 +515,9 @@
       </c>
       <c r="D2" s="5">
         <v>2000</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
       </c>
       <c r="F2" s="7">
         <v>1</v>

</xml_diff>

<commit_message>
- Corrigé un nom de paroisse.
git-svn-id: https://svn.opac.ch/svn/cr/branches/vs2010.1@20635 787ff09c-d2b5-7842-b444-8dd0a418631d
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/App.Aider/Samples/EERV Région 2/id.xlsx
+++ b/Epsitec.Cresus/App.Aider/Samples/EERV Région 2/id.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -48,9 +48,6 @@
     <t>R</t>
   </si>
   <si>
-    <t>Lonay – Préverenges</t>
-  </si>
-  <si>
     <t>L'Aubonne</t>
   </si>
   <si>
@@ -67,6 +64,9 @@
   </si>
   <si>
     <t>Région Morges-Aubonne</t>
+  </si>
+  <si>
+    <t>Lonay – Préverenges – Vullierens</t>
   </si>
 </sst>
 </file>
@@ -472,7 +472,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -517,7 +517,7 @@
         <v>2000</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F2" s="7">
         <v>1</v>
@@ -540,7 +540,7 @@
         <v>2000</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" s="7">
         <v>1</v>
@@ -563,7 +563,7 @@
         <v>2000</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" s="7">
         <v>1</v>
@@ -586,7 +586,7 @@
         <v>2000</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F5" s="7">
         <v>1</v>
@@ -609,7 +609,7 @@
         <v>2000</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6" s="7">
         <v>1</v>
@@ -632,7 +632,7 @@
         <v>2000</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F7" s="7">
         <v>1</v>
@@ -655,7 +655,7 @@
         <v>2000</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F8" s="7">
         <v>1</v>

</xml_diff>